<commit_message>
updated excel sheets and kml for shanghai
Former-commit-id: beaf9501866913c96e6a3686105b31370cb5dc4f
</commit_message>
<xml_diff>
--- a/db/dummydata/new_gc_trucking_shanghai_port.xlsx
+++ b/db/dummydata/new_gc_trucking_shanghai_port.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Zones" sheetId="1" state="visible" r:id="rId2"/>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">NANJING</t>
   </si>
   <si>
-    <t xml:space="preserve">JANGSU</t>
+    <t xml:space="preserve">JIANGSU</t>
   </si>
   <si>
     <t xml:space="preserve">CN</t>
@@ -97,10 +97,10 @@
     <t xml:space="preserve">HUANGSHAN</t>
   </si>
   <si>
-    <t xml:space="preserve">XIAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHANXI</t>
+    <t xml:space="preserve">XI’AN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHAANXI</t>
   </si>
   <si>
     <t xml:space="preserve">CHENGDU</t>
@@ -355,12 +355,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -403,7 +409,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -440,31 +446,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -524,25 +534,24 @@
   <dimension ref="A1:AH999"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="14" min="12" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="18" min="16" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="29" min="20" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="12" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="29" min="20" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -584,7 +593,7 @@
       <c r="B2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -628,7 +637,7 @@
       <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -672,7 +681,7 @@
       <c r="B4" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -716,7 +725,7 @@
       <c r="B5" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -760,7 +769,7 @@
       <c r="B6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -804,7 +813,7 @@
       <c r="B7" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -848,7 +857,7 @@
       <c r="B8" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -892,7 +901,7 @@
       <c r="B9" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -936,7 +945,7 @@
       <c r="B10" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -980,7 +989,7 @@
       <c r="B11" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1024,7 +1033,7 @@
       <c r="B12" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -1338,7 +1347,7 @@
       <c r="D19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="9"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1613,10 +1622,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1698,7 +1707,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="9" t="n">
+      <c r="L2" s="10" t="n">
         <v>250</v>
       </c>
       <c r="M2" s="2"/>
@@ -1733,7 +1742,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="9" t="n">
+      <c r="L3" s="10" t="n">
         <v>450</v>
       </c>
       <c r="M3" s="2"/>
@@ -1766,46 +1775,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="14" t="s">
         <v>67</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -1826,34 +1835,34 @@
       <c r="X1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="15" t="n">
+      <c r="E2" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="12" t="s">
         <v>51</v>
       </c>
       <c r="K2" s="3" t="n">
@@ -1890,23 +1899,23 @@
       <c r="G3" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="18"/>
-      <c r="V3" s="18"/>
-      <c r="W3" s="18"/>
-      <c r="X3" s="18"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
+      <c r="X3" s="19"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
@@ -1930,19 +1939,19 @@
       <c r="G4" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
@@ -1952,37 +1961,37 @@
       <c r="A5" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
+      <c r="B5" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
@@ -1992,620 +2001,620 @@
       <c r="A6" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B6" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="19" t="n">
+      <c r="B6" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="20" t="n">
         <v>0.74</v>
       </c>
-      <c r="D6" s="19" t="n">
+      <c r="D6" s="20" t="n">
         <v>0.7</v>
       </c>
-      <c r="E6" s="20" t="n">
+      <c r="E6" s="21" t="n">
         <v>0.65</v>
       </c>
-      <c r="F6" s="19" t="n">
+      <c r="F6" s="20" t="n">
         <v>0.6</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>145</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="21"/>
-      <c r="W6" s="21"/>
-      <c r="X6" s="21"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="B7" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="19" t="n">
+      <c r="B7" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="20" t="n">
         <v>0.68</v>
       </c>
-      <c r="D7" s="19" t="n">
+      <c r="D7" s="20" t="n">
         <v>0.65</v>
       </c>
-      <c r="E7" s="20" t="n">
+      <c r="E7" s="21" t="n">
         <v>0.6</v>
       </c>
-      <c r="F7" s="19" t="n">
+      <c r="F7" s="20" t="n">
         <v>0.55</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>145</v>
       </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="22"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="B8" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="16" t="n">
+      <c r="B8" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="17" t="n">
         <v>0.68</v>
       </c>
-      <c r="D8" s="16" t="n">
+      <c r="D8" s="17" t="n">
         <v>0.65</v>
       </c>
-      <c r="E8" s="20" t="n">
+      <c r="E8" s="21" t="n">
         <v>0.6</v>
       </c>
-      <c r="F8" s="16" t="n">
+      <c r="F8" s="17" t="n">
         <v>0.55</v>
       </c>
-      <c r="G8" s="16" t="n">
+      <c r="G8" s="17" t="n">
         <v>125</v>
       </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B9" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="16" t="n">
+      <c r="B9" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="17" t="n">
         <v>0.8</v>
       </c>
-      <c r="D9" s="16" t="n">
+      <c r="D9" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="E9" s="20" t="n">
+      <c r="E9" s="21" t="n">
         <v>0.7</v>
       </c>
-      <c r="F9" s="16" t="n">
+      <c r="F9" s="17" t="n">
         <v>0.65</v>
       </c>
-      <c r="G9" s="16" t="n">
+      <c r="G9" s="17" t="n">
         <v>170</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="B10" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="16" t="n">
+      <c r="B10" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="17" t="n">
         <v>0.8</v>
       </c>
-      <c r="D10" s="16" t="n">
+      <c r="D10" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="E10" s="20" t="n">
+      <c r="E10" s="21" t="n">
         <v>0.7</v>
       </c>
-      <c r="F10" s="16" t="n">
+      <c r="F10" s="17" t="n">
         <v>0.65</v>
       </c>
-      <c r="G10" s="16" t="n">
+      <c r="G10" s="17" t="n">
         <v>170</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="B11" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="16" t="n">
+      <c r="B11" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="17" t="n">
         <v>0.92</v>
       </c>
-      <c r="D11" s="16" t="n">
+      <c r="D11" s="17" t="n">
         <v>0.85</v>
       </c>
-      <c r="E11" s="20" t="n">
+      <c r="E11" s="21" t="n">
         <v>0.8</v>
       </c>
-      <c r="F11" s="16" t="n">
+      <c r="F11" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="G11" s="16" t="n">
+      <c r="G11" s="17" t="n">
         <v>160</v>
       </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
+      <c r="T11" s="18"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="B12" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="16" t="n">
+      <c r="B12" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="17" t="n">
         <v>0.8</v>
       </c>
-      <c r="D12" s="16" t="n">
+      <c r="D12" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="E12" s="20" t="n">
+      <c r="E12" s="21" t="n">
         <v>0.7</v>
       </c>
-      <c r="F12" s="16" t="n">
+      <c r="F12" s="17" t="n">
         <v>0.65</v>
       </c>
-      <c r="G12" s="16" t="n">
+      <c r="G12" s="17" t="n">
         <v>120</v>
       </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="18"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="B13" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="16" t="n">
+      <c r="B13" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="17" t="n">
         <v>0.68</v>
       </c>
-      <c r="D13" s="16" t="n">
+      <c r="D13" s="17" t="n">
         <v>0.65</v>
       </c>
-      <c r="E13" s="20" t="n">
+      <c r="E13" s="21" t="n">
         <v>0.6</v>
       </c>
-      <c r="F13" s="16" t="n">
+      <c r="F13" s="17" t="n">
         <v>0.55</v>
       </c>
-      <c r="G13" s="16" t="n">
+      <c r="G13" s="17" t="n">
         <v>130</v>
       </c>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="18"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="B14" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="16" t="n">
+      <c r="B14" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="17" t="n">
         <v>0.48</v>
       </c>
-      <c r="D14" s="16" t="n">
+      <c r="D14" s="17" t="n">
         <v>0.45</v>
       </c>
-      <c r="E14" s="20" t="n">
+      <c r="E14" s="21" t="n">
         <v>0.4</v>
       </c>
-      <c r="F14" s="16" t="n">
+      <c r="F14" s="17" t="n">
         <v>0.35</v>
       </c>
-      <c r="G14" s="16" t="n">
+      <c r="G14" s="17" t="n">
         <v>130</v>
       </c>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="B15" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="16" t="n">
+      <c r="B15" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="17" t="n">
         <v>0.48</v>
       </c>
-      <c r="D15" s="16" t="n">
+      <c r="D15" s="17" t="n">
         <v>0.45</v>
       </c>
-      <c r="E15" s="20" t="n">
+      <c r="E15" s="21" t="n">
         <v>0.4</v>
       </c>
-      <c r="F15" s="16" t="n">
+      <c r="F15" s="17" t="n">
         <v>0.35</v>
       </c>
-      <c r="G15" s="16" t="n">
+      <c r="G15" s="17" t="n">
         <v>135</v>
       </c>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="B16" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="16" t="n">
+      <c r="B16" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="17" t="n">
         <v>0.54</v>
       </c>
-      <c r="D16" s="16" t="n">
+      <c r="D16" s="17" t="n">
         <v>0.5</v>
       </c>
-      <c r="E16" s="20" t="n">
+      <c r="E16" s="21" t="n">
         <v>0.45</v>
       </c>
-      <c r="F16" s="16" t="n">
+      <c r="F16" s="17" t="n">
         <v>0.4</v>
       </c>
-      <c r="G16" s="16" t="n">
+      <c r="G16" s="17" t="n">
         <v>145</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
-      <c r="T16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
+      <c r="S16" s="18"/>
+      <c r="T16" s="18"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="B17" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="16" t="n">
+      <c r="B17" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="17" t="n">
         <v>0.6</v>
       </c>
-      <c r="D17" s="16" t="n">
+      <c r="D17" s="17" t="n">
         <v>0.55</v>
       </c>
-      <c r="E17" s="20" t="n">
+      <c r="E17" s="21" t="n">
         <v>0.5</v>
       </c>
-      <c r="F17" s="16" t="n">
+      <c r="F17" s="17" t="n">
         <v>0.45</v>
       </c>
-      <c r="G17" s="16" t="n">
+      <c r="G17" s="17" t="n">
         <v>150</v>
       </c>
-      <c r="I17" s="16"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="18"/>
+      <c r="T17" s="18"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="B18" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="16" t="n">
+      <c r="B18" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="17" t="n">
         <v>0.72</v>
       </c>
-      <c r="D18" s="16" t="n">
+      <c r="D18" s="17" t="n">
         <v>0.65</v>
       </c>
-      <c r="E18" s="20" t="n">
+      <c r="E18" s="21" t="n">
         <v>0.6</v>
       </c>
-      <c r="F18" s="16" t="n">
+      <c r="F18" s="17" t="n">
         <v>0.55</v>
       </c>
-      <c r="G18" s="16" t="n">
+      <c r="G18" s="17" t="n">
         <v>170</v>
       </c>
-      <c r="I18" s="16"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
-      <c r="T18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="18"/>
+      <c r="T18" s="18"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="B19" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="16" t="n">
+      <c r="B19" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="17" t="n">
         <v>0.8</v>
       </c>
-      <c r="D19" s="16" t="n">
+      <c r="D19" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="E19" s="20" t="n">
+      <c r="E19" s="21" t="n">
         <v>0.7</v>
       </c>
-      <c r="F19" s="16" t="n">
+      <c r="F19" s="17" t="n">
         <v>0.65</v>
       </c>
-      <c r="G19" s="16" t="n">
+      <c r="G19" s="17" t="n">
         <v>170</v>
       </c>
-      <c r="I19" s="16"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="18"/>
+      <c r="T19" s="18"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="B20" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="16" t="n">
+      <c r="B20" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="17" t="n">
         <v>0.92</v>
       </c>
-      <c r="D20" s="16" t="n">
+      <c r="D20" s="17" t="n">
         <v>0.85</v>
       </c>
-      <c r="E20" s="20" t="n">
+      <c r="E20" s="21" t="n">
         <v>0.8</v>
       </c>
-      <c r="F20" s="16" t="n">
+      <c r="F20" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="G20" s="16" t="n">
+      <c r="G20" s="17" t="n">
         <v>210</v>
       </c>
-      <c r="I20" s="16"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
+      <c r="T20" s="18"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="B21" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" s="16" t="n">
+      <c r="B21" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="17" t="n">
         <v>0.86</v>
       </c>
-      <c r="D21" s="16" t="n">
+      <c r="D21" s="17" t="n">
         <v>0.8</v>
       </c>
-      <c r="E21" s="20" t="n">
+      <c r="E21" s="21" t="n">
         <v>0.8</v>
       </c>
-      <c r="F21" s="16" t="n">
+      <c r="F21" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="G21" s="16" t="n">
+      <c r="G21" s="17" t="n">
         <v>190</v>
       </c>
-      <c r="I21" s="16"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="17"/>
-      <c r="S21" s="17"/>
-      <c r="T21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="B22" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" s="16" t="n">
+      <c r="B22" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="17" t="n">
         <v>0.86</v>
       </c>
-      <c r="D22" s="16" t="n">
+      <c r="D22" s="17" t="n">
         <v>0.8</v>
       </c>
-      <c r="E22" s="20" t="n">
+      <c r="E22" s="21" t="n">
         <v>0.8</v>
       </c>
-      <c r="F22" s="16" t="n">
+      <c r="F22" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="G22" s="16" t="n">
+      <c r="G22" s="17" t="n">
         <v>190</v>
       </c>
-      <c r="I22" s="16"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
+      <c r="T22" s="18"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="B23" s="16" t="n">
+      <c r="B23" s="17" t="n">
         <v>0</v>
       </c>
       <c r="C23" s="0" t="n">
@@ -2614,7 +2623,7 @@
       <c r="D23" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="E23" s="20" t="n">
+      <c r="E23" s="21" t="n">
         <v>0.87</v>
       </c>
       <c r="F23" s="0" t="n">
@@ -2623,24 +2632,24 @@
       <c r="G23" s="0" t="n">
         <v>250</v>
       </c>
-      <c r="I23" s="16"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="18"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="B24" s="16" t="n">
+      <c r="B24" s="17" t="n">
         <v>0</v>
       </c>
       <c r="C24" s="0" t="n">
@@ -2649,7 +2658,7 @@
       <c r="D24" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="E24" s="20" t="n">
+      <c r="E24" s="21" t="n">
         <v>1.3</v>
       </c>
       <c r="F24" s="0" t="n">
@@ -2658,22 +2667,22 @@
       <c r="G24" s="0" t="n">
         <v>340</v>
       </c>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="17"/>
-      <c r="T24" s="17"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
+      <c r="T24" s="18"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="B25" s="16" t="n">
+      <c r="B25" s="17" t="n">
         <v>0</v>
       </c>
       <c r="C25" s="0" t="n">
@@ -2682,7 +2691,7 @@
       <c r="D25" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="E25" s="20" t="n">
+      <c r="E25" s="21" t="n">
         <v>1.3</v>
       </c>
       <c r="F25" s="0" t="n">
@@ -2691,22 +2700,22 @@
       <c r="G25" s="0" t="n">
         <v>340</v>
       </c>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="17"/>
-      <c r="S25" s="17"/>
-      <c r="T25" s="17"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="18"/>
+      <c r="T25" s="18"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="n">
         <v>21</v>
       </c>
-      <c r="B26" s="16" t="n">
+      <c r="B26" s="17" t="n">
         <v>0</v>
       </c>
       <c r="C26" s="0" t="n">
@@ -2715,7 +2724,7 @@
       <c r="D26" s="0" t="n">
         <v>0.85</v>
       </c>
-      <c r="E26" s="20" t="n">
+      <c r="E26" s="21" t="n">
         <v>0.8</v>
       </c>
       <c r="F26" s="0" t="n">
@@ -2724,19 +2733,19 @@
       <c r="G26" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="17"/>
-      <c r="R26" s="17"/>
-      <c r="S26" s="17"/>
-      <c r="T26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="18"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2762,52 +2771,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="L1" s="22"/>
+      <c r="L1" s="23"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -2822,40 +2831,40 @@
       <c r="X1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="15" t="n">
+      <c r="E2" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="23" t="n">
+      <c r="K2" s="24" t="n">
         <v>250</v>
       </c>
-      <c r="L2" s="23"/>
+      <c r="L2" s="24"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -2886,23 +2895,23 @@
       <c r="G3" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="18"/>
-      <c r="V3" s="18"/>
-      <c r="W3" s="18"/>
-      <c r="X3" s="18"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
+      <c r="X3" s="19"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
@@ -2926,19 +2935,19 @@
       <c r="G4" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
@@ -2948,37 +2957,37 @@
       <c r="A5" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
+      <c r="B5" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
@@ -2988,620 +2997,620 @@
       <c r="A6" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B6" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="19" t="n">
+      <c r="B6" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="20" t="n">
         <v>0.74</v>
       </c>
-      <c r="D6" s="19" t="n">
+      <c r="D6" s="20" t="n">
         <v>0.7</v>
       </c>
-      <c r="E6" s="20" t="n">
+      <c r="E6" s="21" t="n">
         <v>0.65</v>
       </c>
-      <c r="F6" s="19" t="n">
+      <c r="F6" s="20" t="n">
         <v>0.6</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>145</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="21"/>
-      <c r="W6" s="21"/>
-      <c r="X6" s="21"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="B7" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="19" t="n">
+      <c r="B7" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="20" t="n">
         <v>0.68</v>
       </c>
-      <c r="D7" s="19" t="n">
+      <c r="D7" s="20" t="n">
         <v>0.65</v>
       </c>
-      <c r="E7" s="20" t="n">
+      <c r="E7" s="21" t="n">
         <v>0.6</v>
       </c>
-      <c r="F7" s="19" t="n">
+      <c r="F7" s="20" t="n">
         <v>0.55</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>145</v>
       </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="22"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="B8" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="16" t="n">
+      <c r="B8" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="17" t="n">
         <v>0.68</v>
       </c>
-      <c r="D8" s="16" t="n">
+      <c r="D8" s="17" t="n">
         <v>0.65</v>
       </c>
-      <c r="E8" s="20" t="n">
+      <c r="E8" s="21" t="n">
         <v>0.6</v>
       </c>
-      <c r="F8" s="16" t="n">
+      <c r="F8" s="17" t="n">
         <v>0.55</v>
       </c>
-      <c r="G8" s="16" t="n">
+      <c r="G8" s="17" t="n">
         <v>125</v>
       </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B9" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="16" t="n">
+      <c r="B9" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="17" t="n">
         <v>0.8</v>
       </c>
-      <c r="D9" s="16" t="n">
+      <c r="D9" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="E9" s="20" t="n">
+      <c r="E9" s="21" t="n">
         <v>0.7</v>
       </c>
-      <c r="F9" s="16" t="n">
+      <c r="F9" s="17" t="n">
         <v>0.65</v>
       </c>
-      <c r="G9" s="16" t="n">
+      <c r="G9" s="17" t="n">
         <v>170</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="B10" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="16" t="n">
+      <c r="B10" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="17" t="n">
         <v>0.8</v>
       </c>
-      <c r="D10" s="16" t="n">
+      <c r="D10" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="E10" s="20" t="n">
+      <c r="E10" s="21" t="n">
         <v>0.7</v>
       </c>
-      <c r="F10" s="16" t="n">
+      <c r="F10" s="17" t="n">
         <v>0.65</v>
       </c>
-      <c r="G10" s="16" t="n">
+      <c r="G10" s="17" t="n">
         <v>170</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="B11" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="16" t="n">
+      <c r="B11" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="17" t="n">
         <v>0.92</v>
       </c>
-      <c r="D11" s="16" t="n">
+      <c r="D11" s="17" t="n">
         <v>0.85</v>
       </c>
-      <c r="E11" s="20" t="n">
+      <c r="E11" s="21" t="n">
         <v>0.8</v>
       </c>
-      <c r="F11" s="16" t="n">
+      <c r="F11" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="G11" s="16" t="n">
+      <c r="G11" s="17" t="n">
         <v>160</v>
       </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
+      <c r="T11" s="18"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="B12" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="16" t="n">
+      <c r="B12" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="17" t="n">
         <v>0.8</v>
       </c>
-      <c r="D12" s="16" t="n">
+      <c r="D12" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="E12" s="20" t="n">
+      <c r="E12" s="21" t="n">
         <v>0.7</v>
       </c>
-      <c r="F12" s="16" t="n">
+      <c r="F12" s="17" t="n">
         <v>0.65</v>
       </c>
-      <c r="G12" s="16" t="n">
+      <c r="G12" s="17" t="n">
         <v>120</v>
       </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="18"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="B13" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="16" t="n">
+      <c r="B13" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="17" t="n">
         <v>0.68</v>
       </c>
-      <c r="D13" s="16" t="n">
+      <c r="D13" s="17" t="n">
         <v>0.65</v>
       </c>
-      <c r="E13" s="20" t="n">
+      <c r="E13" s="21" t="n">
         <v>0.6</v>
       </c>
-      <c r="F13" s="16" t="n">
+      <c r="F13" s="17" t="n">
         <v>0.55</v>
       </c>
-      <c r="G13" s="16" t="n">
+      <c r="G13" s="17" t="n">
         <v>130</v>
       </c>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="18"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="B14" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="16" t="n">
+      <c r="B14" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="17" t="n">
         <v>0.48</v>
       </c>
-      <c r="D14" s="16" t="n">
+      <c r="D14" s="17" t="n">
         <v>0.45</v>
       </c>
-      <c r="E14" s="20" t="n">
+      <c r="E14" s="21" t="n">
         <v>0.4</v>
       </c>
-      <c r="F14" s="16" t="n">
+      <c r="F14" s="17" t="n">
         <v>0.35</v>
       </c>
-      <c r="G14" s="16" t="n">
+      <c r="G14" s="17" t="n">
         <v>130</v>
       </c>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="B15" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="16" t="n">
+      <c r="B15" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="17" t="n">
         <v>0.48</v>
       </c>
-      <c r="D15" s="16" t="n">
+      <c r="D15" s="17" t="n">
         <v>0.45</v>
       </c>
-      <c r="E15" s="20" t="n">
+      <c r="E15" s="21" t="n">
         <v>0.4</v>
       </c>
-      <c r="F15" s="16" t="n">
+      <c r="F15" s="17" t="n">
         <v>0.35</v>
       </c>
-      <c r="G15" s="16" t="n">
+      <c r="G15" s="17" t="n">
         <v>135</v>
       </c>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="B16" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="16" t="n">
+      <c r="B16" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="17" t="n">
         <v>0.54</v>
       </c>
-      <c r="D16" s="16" t="n">
+      <c r="D16" s="17" t="n">
         <v>0.5</v>
       </c>
-      <c r="E16" s="20" t="n">
+      <c r="E16" s="21" t="n">
         <v>0.45</v>
       </c>
-      <c r="F16" s="16" t="n">
+      <c r="F16" s="17" t="n">
         <v>0.4</v>
       </c>
-      <c r="G16" s="16" t="n">
+      <c r="G16" s="17" t="n">
         <v>145</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
-      <c r="T16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
+      <c r="S16" s="18"/>
+      <c r="T16" s="18"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="B17" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="16" t="n">
+      <c r="B17" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="17" t="n">
         <v>0.6</v>
       </c>
-      <c r="D17" s="16" t="n">
+      <c r="D17" s="17" t="n">
         <v>0.55</v>
       </c>
-      <c r="E17" s="20" t="n">
+      <c r="E17" s="21" t="n">
         <v>0.5</v>
       </c>
-      <c r="F17" s="16" t="n">
+      <c r="F17" s="17" t="n">
         <v>0.45</v>
       </c>
-      <c r="G17" s="16" t="n">
+      <c r="G17" s="17" t="n">
         <v>150</v>
       </c>
-      <c r="I17" s="16"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="18"/>
+      <c r="T17" s="18"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="B18" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="16" t="n">
+      <c r="B18" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="17" t="n">
         <v>0.72</v>
       </c>
-      <c r="D18" s="16" t="n">
+      <c r="D18" s="17" t="n">
         <v>0.65</v>
       </c>
-      <c r="E18" s="20" t="n">
+      <c r="E18" s="21" t="n">
         <v>0.6</v>
       </c>
-      <c r="F18" s="16" t="n">
+      <c r="F18" s="17" t="n">
         <v>0.55</v>
       </c>
-      <c r="G18" s="16" t="n">
+      <c r="G18" s="17" t="n">
         <v>170</v>
       </c>
-      <c r="I18" s="16"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
-      <c r="T18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="18"/>
+      <c r="T18" s="18"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="B19" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="16" t="n">
+      <c r="B19" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="17" t="n">
         <v>0.8</v>
       </c>
-      <c r="D19" s="16" t="n">
+      <c r="D19" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="E19" s="20" t="n">
+      <c r="E19" s="21" t="n">
         <v>0.7</v>
       </c>
-      <c r="F19" s="16" t="n">
+      <c r="F19" s="17" t="n">
         <v>0.65</v>
       </c>
-      <c r="G19" s="16" t="n">
+      <c r="G19" s="17" t="n">
         <v>170</v>
       </c>
-      <c r="I19" s="16"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="18"/>
+      <c r="T19" s="18"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="B20" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="16" t="n">
+      <c r="B20" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="17" t="n">
         <v>0.92</v>
       </c>
-      <c r="D20" s="16" t="n">
+      <c r="D20" s="17" t="n">
         <v>0.85</v>
       </c>
-      <c r="E20" s="20" t="n">
+      <c r="E20" s="21" t="n">
         <v>0.8</v>
       </c>
-      <c r="F20" s="16" t="n">
+      <c r="F20" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="G20" s="16" t="n">
+      <c r="G20" s="17" t="n">
         <v>210</v>
       </c>
-      <c r="I20" s="16"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
+      <c r="T20" s="18"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="B21" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" s="16" t="n">
+      <c r="B21" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="17" t="n">
         <v>0.86</v>
       </c>
-      <c r="D21" s="16" t="n">
+      <c r="D21" s="17" t="n">
         <v>0.8</v>
       </c>
-      <c r="E21" s="20" t="n">
+      <c r="E21" s="21" t="n">
         <v>0.8</v>
       </c>
-      <c r="F21" s="16" t="n">
+      <c r="F21" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="G21" s="16" t="n">
+      <c r="G21" s="17" t="n">
         <v>190</v>
       </c>
-      <c r="I21" s="16"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="17"/>
-      <c r="S21" s="17"/>
-      <c r="T21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="B22" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" s="16" t="n">
+      <c r="B22" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="17" t="n">
         <v>0.86</v>
       </c>
-      <c r="D22" s="16" t="n">
+      <c r="D22" s="17" t="n">
         <v>0.8</v>
       </c>
-      <c r="E22" s="20" t="n">
+      <c r="E22" s="21" t="n">
         <v>0.8</v>
       </c>
-      <c r="F22" s="16" t="n">
+      <c r="F22" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="G22" s="16" t="n">
+      <c r="G22" s="17" t="n">
         <v>190</v>
       </c>
-      <c r="I22" s="16"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
+      <c r="T22" s="18"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="B23" s="24" t="n">
+      <c r="B23" s="25" t="n">
         <v>0</v>
       </c>
       <c r="C23" s="0" t="n">
@@ -3610,7 +3619,7 @@
       <c r="D23" s="0" t="n">
         <v>0.95</v>
       </c>
-      <c r="E23" s="20" t="n">
+      <c r="E23" s="21" t="n">
         <v>0.87</v>
       </c>
       <c r="F23" s="0" t="n">
@@ -3619,24 +3628,24 @@
       <c r="G23" s="0" t="n">
         <v>250</v>
       </c>
-      <c r="I23" s="16"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="18"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="B24" s="24" t="n">
+      <c r="B24" s="25" t="n">
         <v>0</v>
       </c>
       <c r="C24" s="0" t="n">
@@ -3645,7 +3654,7 @@
       <c r="D24" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="E24" s="20" t="n">
+      <c r="E24" s="21" t="n">
         <v>1.3</v>
       </c>
       <c r="F24" s="0" t="n">
@@ -3654,22 +3663,22 @@
       <c r="G24" s="0" t="n">
         <v>340</v>
       </c>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="17"/>
-      <c r="T24" s="17"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
+      <c r="T24" s="18"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="B25" s="24" t="n">
+      <c r="B25" s="25" t="n">
         <v>0</v>
       </c>
       <c r="C25" s="0" t="n">
@@ -3678,7 +3687,7 @@
       <c r="D25" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="E25" s="20" t="n">
+      <c r="E25" s="21" t="n">
         <v>1.3</v>
       </c>
       <c r="F25" s="0" t="n">
@@ -3687,22 +3696,22 @@
       <c r="G25" s="0" t="n">
         <v>340</v>
       </c>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="17"/>
-      <c r="S25" s="17"/>
-      <c r="T25" s="17"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="18"/>
+      <c r="T25" s="18"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="n">
         <v>21</v>
       </c>
-      <c r="B26" s="24" t="n">
+      <c r="B26" s="25" t="n">
         <v>0</v>
       </c>
       <c r="C26" s="0" t="n">
@@ -3711,7 +3720,7 @@
       <c r="D26" s="0" t="n">
         <v>0.85</v>
       </c>
-      <c r="E26" s="20" t="n">
+      <c r="E26" s="21" t="n">
         <v>0.8</v>
       </c>
       <c r="F26" s="0" t="n">
@@ -3720,19 +3729,19 @@
       <c r="G26" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="17"/>
-      <c r="R26" s="17"/>
-      <c r="S26" s="17"/>
-      <c r="T26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="18"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>